<commit_message>
Filtering received CAN messages due to new motor controller status messages Tweaked object detection logic to improve wall following
</commit_message>
<xml_diff>
--- a/Docs/RCAN.xlsx
+++ b/Docs/RCAN.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="46">
   <si>
     <t>length</t>
   </si>
@@ -28,9 +28,6 @@
   </si>
   <si>
     <t>0,1</t>
-  </si>
-  <si>
-    <t>2,3</t>
   </si>
   <si>
     <t>motor_dIrection_Lf</t>
@@ -147,6 +144,24 @@
   </si>
   <si>
     <t>Right motor speed requested by controller</t>
+  </si>
+  <si>
+    <t>motor_controller_temp_Lf</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>degC</t>
+  </si>
+  <si>
+    <t>Offset</t>
+  </si>
+  <si>
+    <t>motor_controller_temp_Rt</t>
   </si>
 </sst>
 </file>
@@ -170,12 +185,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -190,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -200,6 +221,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -503,34 +527,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:J16"/>
+  <dimension ref="B2:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="11" max="11" width="56.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="1" t="s">
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>0</v>
@@ -542,24 +567,27 @@
         <v>2</v>
       </c>
       <c r="G4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:11" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -570,214 +598,268 @@
       <c r="F5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="I5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="5">
+        <v>16</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="3" t="s">
+      <c r="K6" s="5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="5">
+        <v>16</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="5">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>-273</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:11" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D9" s="2">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="5">
+        <v>16</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="5">
+        <v>16</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="5">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>-273</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4">
+        <v>32</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="4">
+        <v>32</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="2">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="I16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D17" s="2">
+        <v>8</v>
+      </c>
+      <c r="E17" s="2">
+        <v>2</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="2">
+        <v>8</v>
+      </c>
+      <c r="E18" s="2">
         <v>4</v>
       </c>
-      <c r="G6" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="2:10" s="2" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2">
-        <v>2</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2">
-        <v>18</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="4">
-        <v>32</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J11" s="2" t="s">
+      <c r="I18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J18" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="4">
-        <v>32</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="s">
+      <c r="K18" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D15" s="2">
-        <v>8</v>
-      </c>
-      <c r="E15" s="2">
-        <v>2</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="2">
-        <v>8</v>
-      </c>
-      <c r="E16" s="2">
-        <v>4</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>